<commit_message>
TCs and Bug reports
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Reviews .xlsx
+++ b/Monitor and Control/Car-Reviews .xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basma\Desktop\Car-Bookings\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\QA\QA project\Car-Bookings\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42405,8 +42405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42414,7 +42414,7 @@
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>

</xml_diff>